<commit_message>
actualizacion de la estimacion 4ta iteracion de la fase de construccion
</commit_message>
<xml_diff>
--- a/Gestion del Proyecto/Estimacion/Estimacion por CU/Estimaciones/3 ra Estimacion/Proyecto Checkpoint - Estimacion 3.xlsx
+++ b/Gestion del Proyecto/Estimacion/Estimacion por CU/Estimaciones/3 ra Estimacion/Proyecto Checkpoint - Estimacion 3.xlsx
@@ -1659,23 +1659,74 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1704,21 +1755,9 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1743,46 +1782,7 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2094,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K45"/>
   <sheetViews>
-    <sheetView topLeftCell="D24" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="D23" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -2160,11 +2160,11 @@
       <c r="I5" s="43"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
       <c r="F6" s="19">
         <f>Actores!G7</f>
         <v>12</v>
@@ -2173,11 +2173,11 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
       <c r="F7" s="35">
         <f>'Casos De Uso'!F25 -12</f>
         <v>33</v>
@@ -2192,11 +2192,11 @@
       <c r="I9" s="20"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
       <c r="F10" s="19">
         <f>F6+F7</f>
         <v>45</v>
@@ -2223,10 +2223,10 @@
       </c>
     </row>
     <row r="14" spans="2:11" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="102"/>
+      <c r="C14" s="101"/>
       <c r="D14" s="28" t="s">
         <v>18</v>
       </c>
@@ -2452,11 +2452,11 @@
         <v>1</v>
       </c>
       <c r="F24" s="25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G24" s="31">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -2518,39 +2518,39 @@
         <v>1</v>
       </c>
       <c r="F27" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="103"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
       <c r="G28" s="32">
         <f>SUM(G15:G27)</f>
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="103" t="s">
+      <c r="B29" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="103"/>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
-      <c r="F29" s="103"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
       <c r="G29" s="27">
         <f>0.6+(0.01*G28)</f>
-        <v>0.8899999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -2571,10 +2571,10 @@
       <c r="H31" s="36"/>
     </row>
     <row r="32" spans="2:9" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B32" s="102" t="s">
+      <c r="B32" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="102"/>
+      <c r="C32" s="101"/>
       <c r="D32" s="26" t="s">
         <v>6</v>
       </c>
@@ -2608,11 +2608,11 @@
         <v>1.5</v>
       </c>
       <c r="G33" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H33" s="31">
         <f t="shared" ref="H33:H40" si="1">F33*G33</f>
-        <v>6</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="31.5" x14ac:dyDescent="0.2">
@@ -2752,11 +2752,11 @@
         <v>-1</v>
       </c>
       <c r="G39" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H39" s="31">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="78.75" x14ac:dyDescent="0.2">
@@ -2776,39 +2776,39 @@
         <v>-1</v>
       </c>
       <c r="G40" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H40" s="31">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="103" t="s">
+      <c r="B41" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="103"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
-      <c r="F41" s="103"/>
-      <c r="G41" s="103"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
       <c r="H41" s="32">
         <f>SUM(H33:H40)</f>
-        <v>24</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="103" t="s">
+      <c r="B42" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="103"/>
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="103"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="100"/>
       <c r="H42" s="27">
         <f>1.4 + (-0.03*H41)</f>
-        <v>0.67999999999999994</v>
+        <v>0.66499999999999992</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
@@ -2819,31 +2819,31 @@
       <c r="G43" s="24"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="105" t="s">
+      <c r="B45" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="105"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="105"/>
+      <c r="C45" s="102"/>
+      <c r="D45" s="102"/>
+      <c r="E45" s="102"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="102"/>
       <c r="H45" s="40">
         <f>F10*G29*H42</f>
-        <v>27.233999999999995</v>
+        <v>25.436249999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="B28:F28"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="B45:G45"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="B28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2855,7 +2855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -3338,11 +3338,11 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B25" s="34"/>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="104"/>
       <c r="F25" s="35">
         <f>SUM(F3:F24)</f>
         <v>45</v>
@@ -3362,7 +3362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3486,12 +3486,12 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
       <c r="G7" s="19">
         <f>SUM(G3:G6)</f>
         <v>12</v>
@@ -3515,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3530,61 +3530,61 @@
   <sheetData>
     <row r="1" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="129" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="114"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="131"/>
     </row>
     <row r="3" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="127" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="111"/>
+      <c r="C3" s="128"/>
       <c r="D3" s="61" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="125" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="109"/>
+      <c r="C4" s="126"/>
       <c r="D4" s="89">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="107"/>
+      <c r="C5" s="124"/>
       <c r="D5" s="75">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="137" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="125"/>
+      <c r="C6" s="138"/>
       <c r="D6" s="76">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="133" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="121"/>
-      <c r="D8" s="122"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="135"/>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="133" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="123"/>
+      <c r="C9" s="136"/>
       <c r="D9" s="70" t="s">
         <v>113</v>
       </c>
@@ -3636,10 +3636,10 @@
         <f>IF(PCU!G36&lt;3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="128" t="s">
+      <c r="G13" s="108" t="s">
         <v>135</v>
       </c>
-      <c r="H13" s="129"/>
+      <c r="H13" s="141"/>
       <c r="I13" s="95">
         <v>3</v>
       </c>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="D16" s="72">
         <f>IF(PCU!G39&gt;3,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3693,25 +3693,25 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="113" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="118"/>
+      <c r="C18" s="132"/>
       <c r="D18" s="74">
         <f>SUM(D10:D17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="I18" s="115" t="s">
+      <c r="I18" s="106" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="116"/>
-      <c r="K18" s="115" t="s">
+      <c r="J18" s="107"/>
+      <c r="K18" s="106" t="s">
         <v>127</v>
       </c>
-      <c r="L18" s="116"/>
+      <c r="L18" s="107"/>
     </row>
     <row r="19" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H19" s="92" t="s">
@@ -3731,10 +3731,10 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="117" t="s">
+      <c r="B20" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="119"/>
+      <c r="C20" s="114"/>
       <c r="D20" s="77">
         <f>IF($D18&lt;3,20,IF(AND($D18&gt;2,$D18&lt;5),28,IF($D18&gt;4,36,"error")))</f>
         <v>20</v>
@@ -3756,10 +3756,10 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="126" t="s">
+      <c r="G21" s="139" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="127"/>
+      <c r="H21" s="140"/>
       <c r="I21" s="96" t="s">
         <v>136</v>
       </c>
@@ -3777,10 +3777,10 @@
       <c r="B22" s="62"/>
       <c r="C22" s="62"/>
       <c r="D22" s="62"/>
-      <c r="G22" s="128" t="s">
+      <c r="G22" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="H22" s="130"/>
+      <c r="H22" s="110"/>
       <c r="I22" s="96" t="s">
         <v>136</v>
       </c>
@@ -3795,13 +3795,13 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="113" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="119"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="77">
         <f>PCU!H45*'Estimacion h-h'!D20</f>
-        <v>544.67999999999984</v>
+        <v>508.72499999999997</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3810,10 +3810,10 @@
       <c r="D24" s="62"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="131" t="s">
+      <c r="B25" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="132"/>
+      <c r="C25" s="120"/>
       <c r="D25" s="79" t="s">
         <v>119</v>
       </c>
@@ -3822,271 +3822,258 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="133" t="s">
+      <c r="B26" s="121" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="134"/>
+      <c r="C26" s="122"/>
       <c r="D26" s="80">
         <f xml:space="preserve"> ( (( D23*100 ) / 40)*10 ) / 100</f>
-        <v>136.16999999999996</v>
+        <v>127.18125000000001</v>
       </c>
       <c r="E26" s="83">
         <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="135" t="s">
+      <c r="B27" s="117" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="136"/>
+      <c r="C27" s="118"/>
       <c r="D27" s="81">
         <f xml:space="preserve"> ( (( D23*100 ) / 40)*20 ) / 100</f>
-        <v>272.33999999999992</v>
+        <v>254.36250000000001</v>
       </c>
       <c r="E27" s="84">
         <v>0.2</v>
       </c>
-      <c r="I27" s="128" t="s">
+      <c r="I27" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="J27" s="137"/>
-      <c r="K27" s="137"/>
-      <c r="L27" s="130"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="110"/>
     </row>
     <row r="28" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="135" t="s">
+      <c r="B28" s="117" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="136"/>
+      <c r="C28" s="118"/>
       <c r="D28" s="81">
         <f>D23</f>
-        <v>544.67999999999984</v>
+        <v>508.72499999999997</v>
       </c>
       <c r="E28" s="84">
         <v>0.4</v>
       </c>
-      <c r="I28" s="115">
+      <c r="I28" s="106">
         <f>(D31)/4</f>
-        <v>238.2974999999999</v>
-      </c>
-      <c r="J28" s="116"/>
-      <c r="K28" s="115">
+        <v>222.56718749999999</v>
+      </c>
+      <c r="J28" s="107"/>
+      <c r="K28" s="106">
         <f>(D31)/8</f>
-        <v>119.14874999999995</v>
-      </c>
-      <c r="L28" s="116"/>
+        <v>111.28359374999999</v>
+      </c>
+      <c r="L28" s="107"/>
     </row>
     <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="135" t="s">
+      <c r="B29" s="117" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="136"/>
+      <c r="C29" s="118"/>
       <c r="D29" s="81">
         <f xml:space="preserve"> ( (( D23*100 ) / 40)*15 ) / 100</f>
-        <v>204.25499999999994</v>
+        <v>190.77187499999999</v>
       </c>
       <c r="E29" s="84">
         <v>0.15</v>
       </c>
       <c r="I29" s="86">
         <f>I28/22</f>
-        <v>10.83170454545454</v>
+        <v>10.11669034090909</v>
       </c>
       <c r="J29" s="86">
         <f>I28/26</f>
-        <v>9.1652884615384576</v>
+        <v>8.5602764423076927</v>
       </c>
       <c r="K29" s="86">
         <f>K28/22</f>
-        <v>5.4158522727272702</v>
+        <v>5.0583451704545448</v>
       </c>
       <c r="L29" s="86">
         <f>K28/26</f>
-        <v>4.5826442307692288</v>
+        <v>4.2801382211538463</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="138" t="s">
+      <c r="B30" s="111" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="139"/>
+      <c r="C30" s="112"/>
       <c r="D30" s="82">
         <f xml:space="preserve"> ( (( D23*100 ) / 40)*15 ) / 100</f>
-        <v>204.25499999999994</v>
+        <v>190.77187499999999</v>
       </c>
       <c r="E30" s="85">
         <v>0.15</v>
       </c>
       <c r="I30" s="87">
         <f>I29/12</f>
-        <v>0.90264204545454507</v>
+        <v>0.84305752840909076</v>
       </c>
       <c r="J30" s="87">
         <f>J29/12</f>
-        <v>0.76377403846153813</v>
+        <v>0.71335637019230769</v>
       </c>
       <c r="K30" s="87">
         <f>K29/12</f>
-        <v>0.45132102272727254</v>
+        <v>0.42152876420454538</v>
       </c>
       <c r="L30" s="87">
         <f>L29/12</f>
-        <v>0.38188701923076906</v>
+        <v>0.35667818509615384</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="119"/>
-      <c r="D31" s="140">
+      <c r="C31" s="114"/>
+      <c r="D31" s="115">
         <f xml:space="preserve"> SUM( D28:D30 )</f>
-        <v>953.1899999999996</v>
-      </c>
-      <c r="E31" s="141"/>
+        <v>890.26874999999995</v>
+      </c>
+      <c r="E31" s="116"/>
       <c r="I31" s="88">
         <f>I30/I13</f>
-        <v>0.30088068181818167</v>
+        <v>0.28101917613636357</v>
       </c>
       <c r="J31" s="88">
         <f>J30/I13</f>
-        <v>0.25459134615384604</v>
+        <v>0.23778545673076923</v>
       </c>
       <c r="K31" s="88">
         <f>K30/I13</f>
-        <v>0.15044034090909084</v>
+        <v>0.14050958806818178</v>
       </c>
       <c r="L31" s="88">
         <f>L30/I13</f>
-        <v>0.12729567307692302</v>
+        <v>0.11889272836538461</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I32" s="90">
         <f t="shared" ref="I32:K32" si="0">12*I31</f>
-        <v>3.6105681818181798</v>
+        <v>3.3722301136363626</v>
       </c>
       <c r="J32" s="90">
         <f t="shared" si="0"/>
-        <v>3.0550961538461525</v>
+        <v>2.8534254807692307</v>
       </c>
       <c r="K32" s="90">
         <f t="shared" si="0"/>
-        <v>1.8052840909090899</v>
+        <v>1.6861150568181813</v>
       </c>
       <c r="L32" s="90">
         <f>12*L31</f>
-        <v>1.5275480769230763</v>
+        <v>1.4267127403846154</v>
       </c>
     </row>
     <row r="37" spans="9:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="9:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I38" s="128" t="s">
+      <c r="I38" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="J38" s="137"/>
-      <c r="K38" s="137"/>
-      <c r="L38" s="130"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="110"/>
     </row>
     <row r="39" spans="9:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I39" s="115">
+      <c r="I39" s="106">
         <f>(D23)/4</f>
-        <v>136.16999999999996</v>
-      </c>
-      <c r="J39" s="116"/>
-      <c r="K39" s="115">
+        <v>127.18124999999999</v>
+      </c>
+      <c r="J39" s="107"/>
+      <c r="K39" s="106">
         <f>(D23)/8</f>
-        <v>68.08499999999998</v>
-      </c>
-      <c r="L39" s="116"/>
+        <v>63.590624999999996</v>
+      </c>
+      <c r="L39" s="107"/>
     </row>
     <row r="40" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I40" s="86">
         <f>I39/22</f>
-        <v>6.1895454545454527</v>
+        <v>5.7809659090909085</v>
       </c>
       <c r="J40" s="86">
         <f>I39/26</f>
-        <v>5.2373076923076907</v>
+        <v>4.8915865384615378</v>
       </c>
       <c r="K40" s="86">
         <f>K39/22</f>
-        <v>3.0947727272727263</v>
+        <v>2.8904829545454542</v>
       </c>
       <c r="L40" s="86">
         <f>K39/26</f>
-        <v>2.6186538461538453</v>
+        <v>2.4457932692307689</v>
       </c>
     </row>
     <row r="41" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I41" s="87">
         <f>I40/12</f>
-        <v>0.51579545454545439</v>
+        <v>0.48174715909090904</v>
       </c>
       <c r="J41" s="87">
         <f>J40/12</f>
-        <v>0.43644230769230757</v>
+        <v>0.40763221153846146</v>
       </c>
       <c r="K41" s="87">
         <f>K40/12</f>
-        <v>0.2578977272727272</v>
+        <v>0.24087357954545452</v>
       </c>
       <c r="L41" s="87">
         <f>L40/12</f>
-        <v>0.21822115384615379</v>
+        <v>0.20381610576923073</v>
       </c>
     </row>
     <row r="42" spans="9:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I42" s="88">
         <f>I41/I13</f>
-        <v>0.17193181818181813</v>
+        <v>0.16058238636363634</v>
       </c>
       <c r="J42" s="88">
         <f>J41/I13</f>
-        <v>0.14548076923076919</v>
+        <v>0.13587740384615382</v>
       </c>
       <c r="K42" s="88">
         <f>K41/I13</f>
-        <v>8.5965909090909065E-2</v>
+        <v>8.0291193181818168E-2</v>
       </c>
       <c r="L42" s="88">
         <f>L41/I13</f>
-        <v>7.2740384615384596E-2</v>
+        <v>6.7938701923076911E-2</v>
       </c>
     </row>
     <row r="43" spans="9:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I43" s="90">
         <f t="shared" ref="I43:K43" si="1">12*I42</f>
-        <v>2.0631818181818176</v>
+        <v>1.9269886363636362</v>
       </c>
       <c r="J43" s="90">
         <f t="shared" si="1"/>
-        <v>1.7457692307692303</v>
+        <v>1.6305288461538459</v>
       </c>
       <c r="K43" s="90">
         <f t="shared" si="1"/>
-        <v>1.0315909090909088</v>
+        <v>0.96349431818181808</v>
       </c>
       <c r="L43" s="90">
         <f>12*L42</f>
-        <v>0.87288461538461515</v>
+        <v>0.81526442307692293</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
@@ -4103,6 +4090,19 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>